<commit_message>
added more missing column tests
</commit_message>
<xml_diff>
--- a/tests/data/group_variables/group_multiple_sheets.xlsx
+++ b/tests/data/group_variables/group_multiple_sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-data-tools/tests/data/group_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C9DC73-686B-9546-8988-5D53C4792924}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4F5D56-FA9F-8F46-BB60-349ED5814753}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10780" yWindow="3740" windowWidth="23400" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="U3" sqref="U1:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -646,6 +646,9 @@
       <c r="T2">
         <v>0</v>
       </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -673,6 +676,9 @@
         <v>28</v>
       </c>
       <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
         <v>1</v>
       </c>
     </row>

</xml_diff>